<commit_message>
Ver.0.5.21b3. Add hot rolled steel stage.
</commit_message>
<xml_diff>
--- a/resources/design_codes/ГОСТ 8509-93.xlsx
+++ b/resources/design_codes/ГОСТ 8509-93.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uber\IdeaProjects\Armaturkin\resources\design_codes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -74,7 +74,7 @@
     <t>x0, cm</t>
   </si>
   <si>
-    <t>mass per unit length</t>
+    <t>mass per unit length, kg</t>
   </si>
 </sst>
 </file>
@@ -510,7 +510,7 @@
   <dimension ref="A1:Q90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,7 +531,7 @@
     <col min="14" max="14" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>

</xml_diff>